<commit_message>
Correction: Replace bad use of 'converge' with 'process'
According to the supervisor's comments, the use of 'can be converged', 'converge the elements', 'order of convergence' is not known to the English language with the meaning required for the text.
</commit_message>
<xml_diff>
--- a/resources/plot-csv-files/optimizations-50-matrices-double-precision-gp7.xlsx
+++ b/resources/plot-csv-files/optimizations-50-matrices-double-precision-gp7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cejkaluk\git\research-assignment-LU-decomposition\resources\plot-csv-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214AA721-1682-49AC-BFC0-4F26A93721BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09215FBE-4A61-49AF-A336-48CC0D483293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EB188C0A-FAF6-472A-8029-F7F1C455370D}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EB188C0A-FAF6-472A-8029-F7F1C455370D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -218,16 +218,16 @@
     <t>base-diff</t>
   </si>
   <si>
-    <t>computation-row-005-diff</t>
-  </si>
-  <si>
-    <t>computation-row-0-diff</t>
-  </si>
-  <si>
-    <t>computation-row-005-tol</t>
-  </si>
-  <si>
-    <t>computation-row-0-tol</t>
+    <t>processing-row-005-tol</t>
+  </si>
+  <si>
+    <t>processing-row-0-tol</t>
+  </si>
+  <si>
+    <t>processing-row-005-diff</t>
+  </si>
+  <si>
+    <t>processing-row-0-diff</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,10 +620,10 @@
         <v>54</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H1" t="s">
         <v>56</v>
@@ -635,10 +635,10 @@
         <v>59</v>
       </c>
       <c r="K1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M1" t="s">
         <v>55</v>

</xml_diff>